<commit_message>
Updates in package 5
</commit_message>
<xml_diff>
--- a/project/bc/excel/cosmos_bc_model.xlsx
+++ b/project/bc/excel/cosmos_bc_model.xlsx
@@ -597,10 +597,10 @@
   </sheetData>
   <dataValidations count="2">
     <dataValidation sqref="E2:E1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"boolean,decimal,integer,string,uri"</formula1>
+      <formula1>"boolean,date,datetime,decimal,integer,string,uri"</formula1>
     </dataValidation>
     <dataValidation sqref="E2:E1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
-      <formula1>"boolean,decimal,integer,string,uri"</formula1>
+      <formula1>"boolean,date,datetime,decimal,integer,string,uri"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add Package 9 and 10
</commit_message>
<xml_diff>
--- a/project/bc/excel/cosmos_bc_model.xlsx
+++ b/project/bc/excel/cosmos_bc_model.xlsx
@@ -495,17 +495,17 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation sqref="E2:E1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"bc"</formula1>
     </dataValidation>
-    <dataValidation sqref="J2:J1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Quantitative,Ordinal,Nominal,Narrative"</formula1>
+    <dataValidation sqref="J2:J1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Informative,Ordinal,Narrative,Nominal,Quantitative,Temporal"</formula1>
     </dataValidation>
-    <dataValidation sqref="E2:E1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"bc"</formula1>
     </dataValidation>
-    <dataValidation sqref="J2:J1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"Quantitative,Ordinal,Nominal,Narrative"</formula1>
+    <dataValidation sqref="J2:J1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Informative,Ordinal,Narrative,Nominal,Quantitative,Temporal"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -596,11 +596,11 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation sqref="E2:E1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
-      <formula1>"boolean,date,datetime,decimal,integer,string,uri"</formula1>
+    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"boolean,date,datetime,decimal,duration,integer,string,uri"</formula1>
     </dataValidation>
-    <dataValidation sqref="E2:E1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
-      <formula1>"boolean,date,datetime,decimal,integer,string,uri"</formula1>
+    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"boolean,date,datetime,decimal,duration,integer,string,uri"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
initial data collection model
</commit_message>
<xml_diff>
--- a/project/bc/excel/cosmos_bc_model.xlsx
+++ b/project/bc/excel/cosmos_bc_model.xlsx
@@ -429,37 +429,37 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>packageDate</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>packageType</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>BiomedicalConcept_conceptId</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>BiomedicalConcept_ncitCode</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>BiomedicalConcept_href</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>packageDate</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>packageType</t>
-        </is>
-      </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>parentConceptId</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
           <t>categories</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>parentConceptId</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
@@ -495,13 +495,13 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"bc"</formula1>
     </dataValidation>
     <dataValidation sqref="J2:J1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"Ordinal,Narrative,Nominal,Quantitative,Temporal"</formula1>
     </dataValidation>
-    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"bc"</formula1>
     </dataValidation>
     <dataValidation sqref="J2:J1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
@@ -624,37 +624,37 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>packageDate</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>packageType</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>BiomedicalConcept_conceptId</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>BiomedicalConcept_ncitCode</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>BiomedicalConcept_href</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>packageDate</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>packageType</t>
-        </is>
-      </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>parentConceptId</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
           <t>categories</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>parentConceptId</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">

</xml_diff>

<commit_message>
reorganize and add planuml
</commit_message>
<xml_diff>
--- a/project/bc/excel/cosmos_bc_model.xlsx
+++ b/project/bc/excel/cosmos_bc_model.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BiomedicalConcept" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Coding" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataElementConcept" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="BiomedicalConcept" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Coding" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="DataElementConcept" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>